<commit_message>
enhance it to support multiple records
</commit_message>
<xml_diff>
--- a/src/app/app-playloader/sample.xlsx
+++ b/src/app/app-playloader/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeylam/repo/njs/njstool/src/app/app-playloader/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5BBFD7-E59A-8644-9297-241A405F62BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB380DD5-90D8-374D-A3EF-8C1F29AB1981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" xr2:uid="{C145B275-4874-E24D-90F5-C2E9BC1DAA98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Field</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Doe</t>
   </si>
   <si>
-    <t>firstname</t>
-  </si>
-  <si>
     <t>Jane</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>category.2</t>
   </si>
   <si>
-    <t>Technology</t>
-  </si>
-  <si>
     <t>amount</t>
   </si>
   <si>
@@ -89,6 +83,21 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>author.firstname</t>
+  </si>
+  <si>
+    <t>Record-2</t>
+  </si>
+  <si>
+    <t>234-456-2210</t>
+  </si>
+  <si>
+    <t>Shawn</t>
+  </si>
+  <si>
+    <t>Peter</t>
   </si>
 </sst>
 </file>
@@ -440,15 +449,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8E53B1A-C506-0B47-81BD-37026C2C816C}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,10 +465,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -469,10 +481,13 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -480,8 +495,11 @@
       <c r="C3">
         <v>87654321</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -491,49 +509,64 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B8" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
       </c>
       <c r="C8">
         <v>2123.54</v>
+      </c>
+      <c r="D8">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>